<commit_message>
Mini changes Updated coefs
</commit_message>
<xml_diff>
--- a/data/simple/coefficients.xlsx
+++ b/data/simple/coefficients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19321"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B98D0FB1-5135-4BC9-BAE3-6CD2CB321728}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E2064C1-9157-4637-9C73-1586D62A27CC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>id\routes</t>
   </si>
@@ -402,7 +402,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,6 +498,30 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">

</xml_diff>

<commit_message>
coefficients was added and new route.next
</commit_message>
<xml_diff>
--- a/data/simple/coefficients.xlsx
+++ b/data/simple/coefficients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19321"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E2064C1-9157-4637-9C73-1586D62A27CC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{956239D7-D117-4885-94D3-59EB4BE62C17}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
   <si>
     <t>id\routes</t>
   </si>
@@ -47,7 +47,13 @@
     <t>0.125</t>
   </si>
   <si>
-    <t>0.5</t>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.2</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,14 +478,14 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -513,48 +519,216 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="I4">
-        <v>0</v>
+      <c r="I4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
max green time increased new number of state coefs changed cluster updated
</commit_message>
<xml_diff>
--- a/data/simple/coefficients.xlsx
+++ b/data/simple/coefficients.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AF0DD20-D4F7-44FC-843A-B44325ECC3CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{699110B0-F589-4D19-B839-A746660C7F1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="17">
   <si>
     <t>id\routes</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>0.001</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.01</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,6 +802,93 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>